<commit_message>
Added a results storage and simple chart generator, also updated readme
</commit_message>
<xml_diff>
--- a/assets/predictions.xlsx
+++ b/assets/predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,114 +470,114 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>I'm Only Me When I'm With You</t>
+          <t>cardigan</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>So It Goes...</t>
+          <t>Starlight</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Fearless</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The Last Time</t>
+          <t>Speak Now</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Speak Now</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>I Know Places</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>1989</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>I Know Places</t>
+          <t>Mean</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1989</t>
+          <t>Speak Now</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Snow On the Beach</t>
+          <t>False God</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Lover</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>I Think He Knows</t>
+          <t>peace</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -589,12 +589,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>closure</t>
+          <t>august</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>evermore</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -606,58 +606,58 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>I Forgot That You Existed</t>
+          <t>Getaway Car</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>Reputation</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>I Almost Do</t>
+          <t>...Ready for It?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Reputation</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>Reputation</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Blank Space</t>
+          <t>Change</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1989</t>
+          <t>Fearless</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Our Song</t>
+          <t>Tied Together with a Smile</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -667,143 +667,143 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Fearless</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Change</t>
+          <t>no body, no crime</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fearless</t>
+          <t>evermore</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Getaway Car</t>
+          <t>Holy Ground</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>the last great american dynasty</t>
+          <t>Karma</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Midnights</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Maroon</t>
+          <t>Everything Has Changed</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Reputation</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Last Kiss</t>
+          <t>invisible string</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>exile</t>
+          <t>Afterglow</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Lover</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>End Game</t>
+          <t>Out Of The Woods</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>1989</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>Red</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sad Beautiful Tragic</t>
+          <t>Sparks Fly</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Speak Now</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
@@ -820,14 +820,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Lavender Haze</t>
+          <t>Labyrinth</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -837,138 +837,136 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Reputation</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Call It What You Want</t>
+          <t>Better Than Revenge</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Speak Now</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Fearless</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>The Man</t>
+          <t>marjorie</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>evermore</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Fearless</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>the 1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>You're Not Sorry</t>
+          <t>Midnight Rain</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Fearless</t>
+          <t>Midnights</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Don't Blame Me</t>
+          <t>The Outside</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>We Are Never Ever Getting Back Together</t>
+          <t>It's Nice to Have a Friend</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>Lover</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>22</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>Red</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Reputation</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>False God</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Lover</t>
-        </is>
-      </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Reputation</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tim McGraw</t>
+          <t>mirrorball</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -980,46 +978,46 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Gorgeous</t>
+          <t>All Too Well</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>I Did Something Bad</t>
+          <t>The Man</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Lover</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Reputation</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Hey Stephen</t>
+          <t>Invisible</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fearless</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1031,131 +1029,131 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Afterglow</t>
+          <t>long story short</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>evermore</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>Speak Now</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bejeweled</t>
+          <t>Delicate</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Reputation</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Reputation</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mary's Song (Oh My My My)</t>
+          <t>Fifteen</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>Fearless</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>evermore</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>tolerate it</t>
+          <t>this is me trying</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>evermore</t>
+          <t>folklore</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>my tears ricochet</t>
+          <t>Maroon</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Midnights</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>folklore</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Never Grow Up</t>
+          <t>Daylight</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Lover</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Speak Now</t>
+          <t>Fearless</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Begin Again</t>
+          <t>You Need To Calm Down</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Lover</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Fearless</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>The Archer</t>
+          <t>Gorgeous</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Lover</t>
+          <t>Reputation</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1167,51 +1165,799 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>This Is Why We Can't Have Nice Things</t>
+          <t>ivy</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>evermore</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Fearless</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Teardrops On My Guitar</t>
+          <t>Sad Beautiful Tragic</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Midnights</t>
+          <t>Lover</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>White Horse</t>
+          <t>Lavender Haze</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>Midnights</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Our Song</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Enchanted</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Treacherous</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Long Live</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Stay Stay Stay</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Breathe</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>Fearless</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Lover</t>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>All You Had to Do Was Stay</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>This Love</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>The Best Day</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Welcome to New York</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>closure</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>evermore</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Question...?</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Midnights</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Begin Again</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>I Think He Knows</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>evermore</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>evermore</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Haunted</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ME!</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>How You Get The Girl</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>This Is Why We Can't Have Nice Things</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Style</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>End Game</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>dorothea</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>evermore</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Should've Said No</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Anti Hero</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Midnights</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Bejeweled</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Midnights</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>evermore</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>A Place In This World</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>happiness</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>evermore</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Soon You'll Get Better</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>The Archer</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Call It What You Want</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Miss Americana &amp; The Heartbreak Prince</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>You're Not Sorry</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Stay Beautiful</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>State of Grace</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Cold as You</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Never Grow Up</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>hoax</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>folklore</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>epiphany</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>folklore</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>The Way I Loved You</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>seven</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>folklore</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>New Year's Day</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Lover</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>I Did Something Bad</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Speak Now</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Tell Me Why</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Reputation</t>
         </is>
       </c>
     </row>

</xml_diff>